<commit_message>
Fixed courseInfo, course, and grant uploads. Removed job uploads.
</commit_message>
<xml_diff>
--- a/data/courseTemp.xlsx
+++ b/data/courseTemp.xlsx
@@ -375,13 +375,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>department</v>
+      </c>
+      <c r="B1" t="str">
+        <v>number</v>
+      </c>
+      <c r="C1" t="str">
+        <v>univNumber</v>
+      </c>
+      <c r="D1" t="str">
+        <v>name</v>
+      </c>
+      <c r="E1" t="str">
+        <v>category</v>
+      </c>
+      <c r="F1" t="str">
+        <v>topic</v>
+      </c>
+      <c r="G1" t="str">
+        <v>hours</v>
+      </c>
+      <c r="H1" t="str">
+        <v>section</v>
+      </c>
+      <c r="I1" t="str">
+        <v>faculty</v>
+      </c>
+      <c r="J1" t="str">
+        <v>semester</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>COMP</v>
+      </c>
+      <c r="B2" t="str">
+        <v>101</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Fluency in Information Technology</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Theory</v>
+      </c>
+      <c r="F2" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="str">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Ahalt, Stanley</v>
+      </c>
+      <c r="J2" t="str">
+        <v>FA 2018</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>